<commit_message>
Create an aridity index
</commit_message>
<xml_diff>
--- a/landraces_classification/checking_input_data/CIAT_data_counts.xlsx
+++ b/landraces_classification/checking_input_data/CIAT_data_counts.xlsx
@@ -149,7 +149,6 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -157,6 +156,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,7 +440,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -449,406 +451,406 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>23831</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
         <v>15475</v>
       </c>
-      <c r="C3" s="8">
-        <f>B3/B2</f>
+      <c r="C3" s="7">
+        <f>B3/$B$2</f>
         <v>0.64936427342537029</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>715</v>
       </c>
-      <c r="C4" s="8">
-        <f>B4/B2</f>
+      <c r="C4" s="7">
+        <f t="shared" ref="C4:C17" si="0">B4/$B$2</f>
         <v>3.000293735050984E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>7641</v>
       </c>
-      <c r="C5" s="5">
-        <f>B5/B2</f>
+      <c r="C5" s="4">
+        <f t="shared" si="0"/>
         <v>0.32063278922411986</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
         <v>7687</v>
       </c>
-      <c r="C6" s="1">
-        <f>B6/B2</f>
+      <c r="C6" s="8">
+        <f t="shared" si="0"/>
         <v>0.32256304813058623</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>9803</v>
       </c>
-      <c r="C7" s="8">
-        <f>B7/B2</f>
+      <c r="C7" s="7">
+        <f t="shared" si="0"/>
         <v>0.4113549578280391</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>15475</v>
       </c>
-      <c r="C8" s="8">
-        <f>B8/B2</f>
+      <c r="C8" s="7">
+        <f t="shared" si="0"/>
         <v>0.64936427342537029</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>15463</v>
       </c>
-      <c r="C9" s="8">
-        <f>B9/B2</f>
+      <c r="C9" s="7">
+        <f t="shared" si="0"/>
         <v>0.64886072762368341</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>15475</v>
       </c>
-      <c r="C10" s="8">
-        <f>B10/$B$2</f>
+      <c r="C10" s="7">
+        <f t="shared" si="0"/>
         <v>0.64936427342537029</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>15475</v>
       </c>
-      <c r="C11" s="8">
-        <f t="shared" ref="C11:C15" si="0">B11/$B$2</f>
+      <c r="C11" s="7">
+        <f t="shared" si="0"/>
         <v>0.64936427342537029</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>15299</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <f t="shared" si="0"/>
         <v>0.64197893500062941</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>15473</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <f t="shared" si="0"/>
         <v>0.64928034912508914</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>12545</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <f t="shared" si="0"/>
         <v>0.52641517351349087</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>12545</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <f t="shared" si="0"/>
         <v>0.52641517351349087</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>4196</v>
       </c>
-      <c r="C16" s="8">
-        <f>B16/B2</f>
+      <c r="C16" s="7">
+        <f t="shared" si="0"/>
         <v>0.17607318198984517</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>3510</v>
       </c>
-      <c r="C17" s="8">
-        <f>B17/B2</f>
+      <c r="C17" s="7">
+        <f t="shared" si="0"/>
         <v>0.14728714699341194</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="6">
         <v>12545</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="7">
+      <c r="A21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="6">
         <v>12545</v>
       </c>
-      <c r="C21" s="8">
-        <f>B21/B20</f>
+      <c r="C21" s="7">
+        <f>B21/$B$20</f>
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="6">
         <v>0</v>
       </c>
-      <c r="C22" s="8">
-        <f>B22/B20</f>
+      <c r="C22" s="7">
+        <f t="shared" ref="C22:C35" si="1">B22/$B$20</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>0</v>
       </c>
-      <c r="C23" s="5">
-        <f>B23/B20</f>
+      <c r="C23" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B24">
         <v>7687</v>
       </c>
-      <c r="C24" s="1">
-        <f>B24/B20</f>
+      <c r="C24" s="8">
+        <f t="shared" si="1"/>
         <v>0.61275408529294539</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="6">
         <v>7780</v>
       </c>
-      <c r="C25" s="8">
-        <f>B25/B20</f>
+      <c r="C25" s="7">
+        <f t="shared" si="1"/>
         <v>0.62016739736946991</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="6">
         <v>12545</v>
       </c>
-      <c r="C26" s="8">
-        <f>B26/B20</f>
+      <c r="C26" s="7">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="6">
         <v>12534</v>
       </c>
-      <c r="C27" s="8">
-        <f>B27/B20</f>
+      <c r="C27" s="7">
+        <f t="shared" si="1"/>
         <v>0.99912315663610995</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="6">
         <v>12545</v>
       </c>
-      <c r="C28" s="8">
-        <f>B28/$B$2</f>
-        <v>0.52641517351349087</v>
+      <c r="C28" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="6">
         <v>12545</v>
       </c>
-      <c r="C29" s="8">
-        <f t="shared" ref="C29:C33" si="1">B29/$B$2</f>
-        <v>0.52641517351349087</v>
+      <c r="C29" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="6">
         <v>12392</v>
       </c>
-      <c r="C30" s="8">
-        <f t="shared" si="1"/>
-        <v>0.51999496454198313</v>
+      <c r="C30" s="7">
+        <f t="shared" si="1"/>
+        <v>0.987803905938621</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="6">
         <v>12543</v>
       </c>
-      <c r="C31" s="8">
-        <f t="shared" si="1"/>
-        <v>0.52633124921320973</v>
+      <c r="C31" s="7">
+        <f t="shared" si="1"/>
+        <v>0.99984057393383818</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="6">
         <v>12545</v>
       </c>
-      <c r="C32" s="8">
-        <f t="shared" si="1"/>
-        <v>0.52641517351349087</v>
+      <c r="C32" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="6">
         <v>12545</v>
       </c>
-      <c r="C33" s="8">
-        <f t="shared" si="1"/>
-        <v>0.52641517351349087</v>
+      <c r="C33" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="7">
+      <c r="B34" s="6">
         <v>3000</v>
       </c>
-      <c r="C34" s="8">
-        <f>B34/B20</f>
+      <c r="C34" s="7">
+        <f t="shared" si="1"/>
         <v>0.23913909924272619</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B35" s="7">
+      <c r="B35" s="6">
         <v>3000</v>
       </c>
-      <c r="C35" s="8">
-        <f>B35/B20</f>
+      <c r="C35" s="7">
+        <f t="shared" si="1"/>
         <v>0.23913909924272619</v>
       </c>
     </row>

</xml_diff>